<commit_message>
Update trading results - Wed Sep 10 13:49:29 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,88 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-09-10T13:49:26.889804</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>113902.0791768574</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-09-10T13:49:28.786247</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>113902.0791768574</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9600</v>
+      </c>
+      <c r="G3" t="n">
+        <v>40</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.714390973461102</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Sep 19 19:27:01 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,6 +577,240 @@
       </c>
       <c r="L3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:26:56.251149</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3.115658833304698</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:26:57.769743</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:26:57.782292</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>3.66429971981016</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:26:59.211472</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:26:59.224981</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8963706973452196</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:27:00.824559</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Sep 19 19:35:14 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -811,6 +811,244 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:35:09.642979</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>3.119850135476197</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:35:11.142328</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>3.119850135476197</v>
+      </c>
+      <c r="F11" t="n">
+        <v>120</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:35:11.155401</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>3.665685532018927</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:35:12.737999</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:35:12.752205</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8978693919281808</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:35:14.350933</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Sep 19 19:57:25 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1049,6 +1049,244 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:57:19.335693</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>3.123607372056906</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:57:21.426956</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>3.123607372056906</v>
+      </c>
+      <c r="F17" t="n">
+        <v>120</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:57:21.442593</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>3.655574672649196</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:57:23.136489</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:57:23.152748</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0.8960502649311237</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-09-19T19:57:24.887649</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sat Sep 20 01:23:09 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,6 +1287,88 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-09-20T01:23:07.266452</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0.6727811902747289</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-09-20T01:23:08.787988</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0.6727811902747289</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.6326121610267794</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sat Sep 20 12:39:24 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1369,6 +1369,88 @@
       </c>
       <c r="L23" t="inlineStr"/>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-09-20T12:39:21.948063</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0.6727811902747289</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-09-20T12:39:23.406345</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0.6727811902747289</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G25" t="n">
+        <v>10</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.07577367435598509</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Sep 22 01:32:00 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1451,6 +1451,252 @@
       </c>
       <c r="L25" t="inlineStr"/>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-09-22T01:31:54.822615</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>236.6486785425042</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-09-22T01:31:56.476164</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>236.6486785425042</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.09115590152285132</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-09-22T01:31:56.494749</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>115304.4799940704</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-09-22T01:31:58.040397</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>115304.4799940704</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4800</v>
+      </c>
+      <c r="G29" t="n">
+        <v>40</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.2552237794056823</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-09-22T01:31:58.059394</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0.6448516400994989</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-09-22T01:31:59.674594</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0.6448516400994989</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>10</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.301833833851505</v>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Sep 22 12:43:50 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1697,6 +1697,170 @@
       </c>
       <c r="L31" t="inlineStr"/>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-09-22T12:43:46.357167</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>2.973349691321248</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-09-22T12:43:48.480932</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>2.973349691321248</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.03925898863075103</v>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-09-22T12:43:48.500959</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0.6448516400994989</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-09-22T12:43:50.177958</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0.6448516400994989</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G35" t="n">
+        <v>10</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.544849307081386</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Sep 23 01:25:29 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1861,6 +1861,248 @@
       </c>
       <c r="L35" t="inlineStr"/>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-09-23T01:25:25.131648</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0.4364983524810095</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-09-23T01:25:27.195967</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0.4364983524810095</v>
+      </c>
+      <c r="F37" t="n">
+        <v>900</v>
+      </c>
+      <c r="G37" t="n">
+        <v>10</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.125864799809103</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-09-23T01:25:27.217209</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>2.851139194678168</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-09-23T01:25:28.902338</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>2.851139194678168</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G39" t="n">
+        <v>20</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.1159561015951102</v>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-09-23T01:25:28.923622</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0.6000566049103071</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-09-23T01:25:29.117100</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Sep 23 06:53:52 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2103,6 +2103,88 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-09-23T06:53:49.541389</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0.6000566049103071</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-09-23T06:53:51.349247</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0.6000566049103071</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G43" t="n">
+        <v>10</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.8506466283814236</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Sep 25 01:26:52 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2185,6 +2185,170 @@
       </c>
       <c r="L43" t="inlineStr"/>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-09-25T01:26:48.157640</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>210.841151833073</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-09-25T01:26:49.937087</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>210.841151833073</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G45" t="n">
+        <v>20</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.4434054849163298</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-09-25T01:26:49.962191</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>3.348909889983477</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-09-25T01:26:51.589220</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>3.348909889983477</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G47" t="n">
+        <v>10</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.6539174731116587</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Sep 25 12:43:57 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2349,6 +2349,84 @@
       </c>
       <c r="L47" t="inlineStr"/>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:43:56.425956</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>211.5960881268497</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:43:56.817993</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Sep 26 01:26:14 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2427,6 +2427,170 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-09-26T01:26:10.864062</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0.4151322031279097</v>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-09-26T01:26:12.398565</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>0.4151322031279097</v>
+      </c>
+      <c r="F51" t="n">
+        <v>900</v>
+      </c>
+      <c r="G51" t="n">
+        <v>10</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.006277752397636782</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-09-26T01:26:12.422759</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>0.5806741401362351</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-09-26T01:26:13.932688</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0.5806741401362351</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G53" t="n">
+        <v>10</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1.054574706292496</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Sep 29 01:28:02 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2591,6 +2591,88 @@
       </c>
       <c r="L53" t="inlineStr"/>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-09-29T01:28:00.101981</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>112265.3486426338</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-09-29T01:28:01.747841</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>112265.3486426338</v>
+      </c>
+      <c r="F55" t="n">
+        <v>3600</v>
+      </c>
+      <c r="G55" t="n">
+        <v>40</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.2775619584775681</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Oct  3 01:24:20 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2673,6 +2673,84 @@
       </c>
       <c r="L55" t="inlineStr"/>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-10-03T01:24:18.031794</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>3.546780152288974</v>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-10-03T01:24:19.927512</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Oct  3 12:42:01 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2751,6 +2751,84 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-10-03T12:41:58.629075</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>3.582294139231992</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-10-03T12:42:00.542078</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sat Oct  4 01:22:28 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2829,6 +2829,634 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:14.291475</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>231.386880157209</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:16.169141</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:16.196986</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>122145.0094321105</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:17.935069</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>122145.0094321105</v>
+      </c>
+      <c r="F63" t="n">
+        <v>90</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:17.961778</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>4492.563675941279</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:19.648871</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:19.677577</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>0.4475369841415226</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Attempting trade 4/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:21.331050</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:21.361777</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>3.580526691599361</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Attempting trade 5/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:23.144754</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:23.174530</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>3.037337837354311</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Attempting trade 6/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:24.790784</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:24.820697</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>289.7331155048397</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Attempting trade 7/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:26.497201</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:26.526928</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>0.6116338841784414</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Attempting trade 8/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-10-04T01:22:28.293407</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 8</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sat Oct  4 12:38:40 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3457,6 +3457,552 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:26.997476</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>233.064580246805</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:28.975269</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:29.008107</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>122250.151868428</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:30.745560</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:30.778527</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>4515.759068159723</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:32.474841</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:32.507311</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>0.4505143051833715</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Attempting trade 4/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:34.377397</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:34.412320</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>3.582136289260382</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Attempting trade 5/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:36.296444</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:36.331327</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>3.041366390190445</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Attempting trade 6/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:38.148810</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:38.183243</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>290.9949382388142</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Attempting trade 7/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-10-04T12:38:40.071041</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Oct 20 01:33:32 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4003,6 +4003,88 @@
         </is>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-10-20T01:33:30.469956</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>0.3208392693959338</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-10-20T01:33:32.061100</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>0.3208392693959338</v>
+      </c>
+      <c r="F91" t="n">
+        <v>900</v>
+      </c>
+      <c r="G91" t="n">
+        <v>10</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.1367964106814732</v>
+      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Oct 20 12:44:53 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L91"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4085,6 +4085,88 @@
       </c>
       <c r="L91" t="inlineStr"/>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-10-20T12:44:52.001924</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>108621.134857428</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-10-20T12:44:53.326525</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>108621.134857428</v>
+      </c>
+      <c r="F93" t="n">
+        <v>3600</v>
+      </c>
+      <c r="G93" t="n">
+        <v>40</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.08208394928824908</v>
+      </c>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Oct 23 01:29:05 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4167,6 +4167,88 @@
       </c>
       <c r="L93" t="inlineStr"/>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-10-23T01:29:03.723353</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>0.3222621896511093</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-10-23T01:29:05.338613</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>0.3222621896511093</v>
+      </c>
+      <c r="F95" t="n">
+        <v>90</v>
+      </c>
+      <c r="G95" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Oct 23 12:43:41 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4249,6 +4249,88 @@
       </c>
       <c r="L95" t="inlineStr"/>
     </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-10-23T12:43:39.553291</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>0.3220488363629825</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-10-23T12:43:41.235374</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>0.3220488363629825</v>
+      </c>
+      <c r="F97" t="n">
+        <v>90</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Oct 28 01:28:09 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4331,6 +4331,84 @@
       </c>
       <c r="L97" t="inlineStr"/>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-10-28T01:28:07.082034</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>4128.421039015593</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-10-28T01:28:08.970846</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Oct 28 12:44:33 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4409,6 +4409,84 @@
         </is>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-10-28T12:44:30.584659</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>4123.206220671679</v>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-10-28T12:44:32.730295</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sun Nov  9 01:42:43 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4487,6 +4487,84 @@
         </is>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-11-09T01:42:41.703833</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>200.8622597986005</v>
+      </c>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-11-09T01:42:43.221998</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Nov 10 01:44:07 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4565,6 +4565,330 @@
         </is>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:01.184016</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>105810.2124022901</v>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:02.527362</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>105810.2124022901</v>
+      </c>
+      <c r="F105" t="n">
+        <v>3600</v>
+      </c>
+      <c r="G105" t="n">
+        <v>40</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.5304736892722409</v>
+      </c>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:02.565645</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>2.915819709647294</v>
+      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:03.891119</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:03.942391</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>2.401335169398255</v>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:05.108886</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>2.401335169398255</v>
+      </c>
+      <c r="F109" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G109" t="n">
+        <v>20</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.3424941803961721</v>
+      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:05.148365</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>0.3440884159654859</v>
+      </c>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>Attempting trade 4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-11-10T01:44:06.376962</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>0.3440884159654859</v>
+      </c>
+      <c r="F111" t="n">
+        <v>900</v>
+      </c>
+      <c r="G111" t="n">
+        <v>10</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.4929621216371939</v>
+      </c>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Nov 10 12:45:32 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L111"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4889,6 +4889,84 @@
       </c>
       <c r="L111" t="inlineStr"/>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-11-10T12:45:30.826576</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>3.034482039611791</v>
+      </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-11-10T12:45:32.286401</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>NEAR</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Wed Nov 19 01:30:01 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L113"/>
+  <dimension ref="A1:L115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4967,6 +4967,84 @@
         </is>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-11-19T01:29:59.570598</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>0.1609846586716453</v>
+      </c>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-11-19T01:30:01.143677</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Wed Nov 19 12:46:14 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5045,6 +5045,84 @@
         </is>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-11-19T12:46:12.008162</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>0.161571559273133</v>
+      </c>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-11-19T12:46:13.585123</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Nov 24 01:46:55 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5123,6 +5123,88 @@
         </is>
       </c>
     </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-11-24T01:46:53.132304</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>86576.78246280954</v>
+      </c>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-11-24T01:46:54.474317</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>86576.78246280954</v>
+      </c>
+      <c r="F119" t="n">
+        <v>3600</v>
+      </c>
+      <c r="G119" t="n">
+        <v>40</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0.3108185808726259</v>
+      </c>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Nov 25 01:32:33 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5205,6 +5205,84 @@
       </c>
       <c r="L119" t="inlineStr"/>
     </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-11-25T01:32:30.772939</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>0.4275831039888888</v>
+      </c>
+      <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-11-25T01:32:32.315612</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Nov 28 01:30:30 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L121"/>
+  <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5283,6 +5283,84 @@
         </is>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-11-28T01:30:29.457443</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>0.2800772548903293</v>
+      </c>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-11-28T01:30:29.755545</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Nov 28 12:45:31 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L123"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5361,6 +5361,84 @@
         </is>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-11-28T12:45:30.072511</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>0.2802319893231524</v>
+      </c>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-11-28T12:45:30.292195</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Dec  4 01:41:54 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L125"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5439,6 +5439,84 @@
         </is>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-12-04T01:41:51.952548</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>93511.79991045169</v>
+      </c>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-12-04T01:41:53.536618</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Dec  4 12:46:59 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5517,6 +5517,84 @@
         </is>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-12-04T12:46:57.289943</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>93619.43750817103</v>
+      </c>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-12-04T12:46:58.950964</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Dec 11 01:46:21 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5595,6 +5595,162 @@
         </is>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-12-11T01:46:17.236707</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>133.5144301747269</v>
+      </c>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-12-11T01:46:18.963429</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-12-11T01:46:19.008333</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>3267.627119741301</v>
+      </c>
+      <c r="F132" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-12-11T01:46:20.481552</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Dec 11 12:48:03 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L133"/>
+  <dimension ref="A1:L135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5751,6 +5751,84 @@
         </is>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-12-11T12:48:00.195463</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>3326.260211637518</v>
+      </c>
+      <c r="F134" t="inlineStr"/>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr"/>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-12-11T12:48:02.297621</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Dec 19 12:46:00 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L135"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5829,6 +5829,88 @@
         </is>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-12-19T12:45:58.854607</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>0.1971157803419345</v>
+      </c>
+      <c r="F136" t="inlineStr"/>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-12-19T12:46:00.245794</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>0.1971157803419345</v>
+      </c>
+      <c r="F137" t="n">
+        <v>900</v>
+      </c>
+      <c r="G137" t="n">
+        <v>10</v>
+      </c>
+      <c r="H137" t="n">
+        <v>0.04858655748916241</v>
+      </c>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sat Dec 20 01:32:31 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L137"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5911,6 +5911,244 @@
       </c>
       <c r="L137" t="inlineStr"/>
     </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-12-20T01:32:25.745125</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>1.902841385919959</v>
+      </c>
+      <c r="F138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-12-20T01:32:27.330466</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-12-20T01:32:27.377495</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>0.2088469583591241</v>
+      </c>
+      <c r="F140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr"/>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-12-20T01:32:28.924836</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>0.2088469583591241</v>
+      </c>
+      <c r="F141" t="n">
+        <v>90</v>
+      </c>
+      <c r="G141" t="n">
+        <v>1</v>
+      </c>
+      <c r="H141" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr"/>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-12-20T01:32:28.971842</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>0.1309857893276292</v>
+      </c>
+      <c r="F142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" t="inlineStr"/>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-12-20T01:32:30.463587</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sat Dec 20 12:42:55 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6149,6 +6149,88 @@
         </is>
       </c>
     </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-12-20T12:42:53.612503</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>0.2090737778061083</v>
+      </c>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" t="inlineStr"/>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-12-20T12:42:54.895196</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>0.2090737778061083</v>
+      </c>
+      <c r="F145" t="n">
+        <v>90</v>
+      </c>
+      <c r="G145" t="n">
+        <v>1</v>
+      </c>
+      <c r="H145" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Dec 22 01:50:54 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6231,6 +6231,88 @@
       </c>
       <c r="L145" t="inlineStr"/>
     </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-12-22T01:50:52.187427</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>0.2158159392036846</v>
+      </c>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-12-22T01:50:53.486200</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>0.2158159392036846</v>
+      </c>
+      <c r="F147" t="n">
+        <v>900</v>
+      </c>
+      <c r="G147" t="n">
+        <v>10</v>
+      </c>
+      <c r="H147" t="n">
+        <v>0.1878546736117281</v>
+      </c>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" t="inlineStr"/>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Fri Dec 26 01:46:19 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L147"/>
+  <dimension ref="A1:L149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6313,6 +6313,88 @@
       </c>
       <c r="L147" t="inlineStr"/>
     </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-12-26T01:46:17.546101</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>150.3296743373134</v>
+      </c>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-12-26T01:46:18.901603</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>150.3296743373134</v>
+      </c>
+      <c r="F149" t="n">
+        <v>900</v>
+      </c>
+      <c r="G149" t="n">
+        <v>10</v>
+      </c>
+      <c r="H149" t="n">
+        <v>0.5775886465174159</v>
+      </c>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L149" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Dec 29 01:52:57 UTC 2025
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L149"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6395,6 +6395,88 @@
       </c>
       <c r="L149" t="inlineStr"/>
     </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-12-29T01:52:55.811345</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>129.1026777995603</v>
+      </c>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-12-29T01:52:57.159731</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>129.1026777995603</v>
+      </c>
+      <c r="F151" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G151" t="n">
+        <v>20</v>
+      </c>
+      <c r="H151" t="n">
+        <v>0.8257117870327627</v>
+      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Sun Jan  4 12:45:03 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L151"/>
+  <dimension ref="A1:L153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6477,6 +6477,84 @@
       </c>
       <c r="L151" t="inlineStr"/>
     </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-01-04T12:45:01.334547</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>2.017506273157977</v>
+      </c>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-01-04T12:45:03.068627</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Jan  5 01:55:55 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L153"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6555,6 +6555,166 @@
         </is>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-01-05T01:55:52.741161</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>93117.57494500774</v>
+      </c>
+      <c r="F154" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-01-05T01:55:54.403711</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>93117.57494500774</v>
+      </c>
+      <c r="F155" t="n">
+        <v>7200</v>
+      </c>
+      <c r="G155" t="n">
+        <v>40</v>
+      </c>
+      <c r="H155" t="n">
+        <v>1.681936884743757</v>
+      </c>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-01-05T01:55:54.448482</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>3204.677318622782</v>
+      </c>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="inlineStr"/>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2026-01-05T01:55:54.682973</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="inlineStr"/>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Jan  5 12:51:14 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L157"/>
+  <dimension ref="A1:L159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6715,6 +6715,84 @@
         </is>
       </c>
     </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2026-01-05T12:51:13.855680</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>1.690107061821174</v>
+      </c>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="inlineStr"/>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2026-01-05T12:51:14.036393</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="inlineStr"/>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="inlineStr"/>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Jan  6 01:49:20 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L159"/>
+  <dimension ref="A1:L163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6793,6 +6793,162 @@
         </is>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2026-01-06T01:49:18.823736</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>0.2530262800374813</v>
+      </c>
+      <c r="F160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2026-01-06T01:49:19.289596</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" t="inlineStr"/>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2026-01-06T01:49:19.342395</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>0.1520220401133235</v>
+      </c>
+      <c r="F162" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" t="inlineStr"/>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2026-01-06T01:49:19.664392</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" t="inlineStr"/>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Jan  6 12:47:01 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L163"/>
+  <dimension ref="A1:L167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6949,6 +6949,162 @@
         </is>
       </c>
     </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2026-01-06T12:47:00.521657</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>0.2537161193615907</v>
+      </c>
+      <c r="F164" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" t="inlineStr"/>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2026-01-06T12:47:00.749178</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" t="inlineStr"/>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2026-01-06T12:47:00.801470</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>0.1519393256021509</v>
+      </c>
+      <c r="F166" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" t="inlineStr"/>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2026-01-06T12:47:01.125724</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr"/>
+      <c r="F167" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" t="inlineStr"/>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Wed Jan  7 01:48:51 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L167"/>
+  <dimension ref="A1:L171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7105,6 +7105,162 @@
         </is>
       </c>
     </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2026-01-07T01:48:47.401656</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>3246.247548899048</v>
+      </c>
+      <c r="F168" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" t="inlineStr"/>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2026-01-07T01:48:48.952047</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" t="inlineStr"/>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2026-01-07T01:48:49.006777</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>1.861190696770879</v>
+      </c>
+      <c r="F170" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+      <c r="J170" t="inlineStr"/>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2026-01-07T01:48:51.004658</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr"/>
+      <c r="F171" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" t="inlineStr"/>
+      <c r="I171" t="inlineStr"/>
+      <c r="J171" t="inlineStr"/>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Wed Jan  7 12:50:06 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L171"/>
+  <dimension ref="A1:L173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7261,6 +7261,84 @@
         </is>
       </c>
     </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2026-01-07T12:50:04.591130</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>1.905757779236831</v>
+      </c>
+      <c r="F172" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" t="inlineStr"/>
+      <c r="I172" t="inlineStr"/>
+      <c r="J172" t="inlineStr"/>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2026-01-07T12:50:06.136738</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>SUI</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr"/>
+      <c r="F173" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+      <c r="J173" t="inlineStr"/>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Mon Jan 12 01:54:27 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L173"/>
+  <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7339,6 +7339,88 @@
         </is>
       </c>
     </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2026-01-12T01:54:25.597482</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>141.1500030432715</v>
+      </c>
+      <c r="F174" t="inlineStr"/>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" t="inlineStr"/>
+      <c r="I174" t="inlineStr"/>
+      <c r="J174" t="inlineStr"/>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2026-01-12T01:54:26.922051</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>POSITION_OPENED</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>141.1500030432715</v>
+      </c>
+      <c r="F175" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G175" t="n">
+        <v>20</v>
+      </c>
+      <c r="H175" t="n">
+        <v>0.09385894641150276</v>
+      </c>
+      <c r="I175" t="inlineStr"/>
+      <c r="J175" t="inlineStr"/>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Wed Jan 14 01:53:26 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L175"/>
+  <dimension ref="A1:L177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7421,6 +7421,84 @@
       </c>
       <c r="L175" t="inlineStr"/>
     </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2026-01-14T01:53:24.279390</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>0.3044672549109288</v>
+      </c>
+      <c r="F176" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" t="inlineStr"/>
+      <c r="I176" t="inlineStr"/>
+      <c r="J176" t="inlineStr"/>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2026-01-14T01:53:25.632389</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr"/>
+      <c r="F177" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" t="inlineStr"/>
+      <c r="I177" t="inlineStr"/>
+      <c r="J177" t="inlineStr"/>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Jan 15 01:48:36 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L177"/>
+  <dimension ref="A1:L191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7499,6 +7499,552 @@
         </is>
       </c>
     </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:23.859094</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>145.1279744138415</v>
+      </c>
+      <c r="F178" t="inlineStr"/>
+      <c r="G178" t="inlineStr"/>
+      <c r="H178" t="inlineStr"/>
+      <c r="I178" t="inlineStr"/>
+      <c r="J178" t="inlineStr"/>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:25.396659</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" t="inlineStr"/>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" t="inlineStr"/>
+      <c r="I179" t="inlineStr"/>
+      <c r="J179" t="inlineStr"/>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:25.456699</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>3327.551283719895</v>
+      </c>
+      <c r="F180" t="inlineStr"/>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" t="inlineStr"/>
+      <c r="I180" t="inlineStr"/>
+      <c r="J180" t="inlineStr"/>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>Attempting trade 2/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:27.168094</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr"/>
+      <c r="F181" t="inlineStr"/>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" t="inlineStr"/>
+      <c r="I181" t="inlineStr"/>
+      <c r="J181" t="inlineStr"/>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:27.226546</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>0.216980312763392</v>
+      </c>
+      <c r="F182" t="inlineStr"/>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr"/>
+      <c r="I182" t="inlineStr"/>
+      <c r="J182" t="inlineStr"/>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>Attempting trade 3/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:28.808707</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>ARB</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr"/>
+      <c r="F183" t="inlineStr"/>
+      <c r="G183" t="inlineStr"/>
+      <c r="H183" t="inlineStr"/>
+      <c r="I183" t="inlineStr"/>
+      <c r="J183" t="inlineStr"/>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:28.867842</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>176.5633354836947</v>
+      </c>
+      <c r="F184" t="inlineStr"/>
+      <c r="G184" t="inlineStr"/>
+      <c r="H184" t="inlineStr"/>
+      <c r="I184" t="inlineStr"/>
+      <c r="J184" t="inlineStr"/>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>Attempting trade 4/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:30.614313</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr"/>
+      <c r="F185" t="inlineStr"/>
+      <c r="G185" t="inlineStr"/>
+      <c r="H185" t="inlineStr"/>
+      <c r="I185" t="inlineStr"/>
+      <c r="J185" t="inlineStr"/>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:30.678715</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>0.4092984782323901</v>
+      </c>
+      <c r="F186" t="inlineStr"/>
+      <c r="G186" t="inlineStr"/>
+      <c r="H186" t="inlineStr"/>
+      <c r="I186" t="inlineStr"/>
+      <c r="J186" t="inlineStr"/>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>Attempting trade 5/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:32.292888</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr"/>
+      <c r="F187" t="inlineStr"/>
+      <c r="G187" t="inlineStr"/>
+      <c r="H187" t="inlineStr"/>
+      <c r="I187" t="inlineStr"/>
+      <c r="J187" t="inlineStr"/>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:32.353612</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>0.235081410141356</v>
+      </c>
+      <c r="F188" t="inlineStr"/>
+      <c r="G188" t="inlineStr"/>
+      <c r="H188" t="inlineStr"/>
+      <c r="I188" t="inlineStr"/>
+      <c r="J188" t="inlineStr"/>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>Attempting trade 6/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:33.839931</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>ENA</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr"/>
+      <c r="F189" t="inlineStr"/>
+      <c r="G189" t="inlineStr"/>
+      <c r="H189" t="inlineStr"/>
+      <c r="I189" t="inlineStr"/>
+      <c r="J189" t="inlineStr"/>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:33.900460</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>0.144971116122147</v>
+      </c>
+      <c r="F190" t="inlineStr"/>
+      <c r="G190" t="inlineStr"/>
+      <c r="H190" t="inlineStr"/>
+      <c r="I190" t="inlineStr"/>
+      <c r="J190" t="inlineStr"/>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>Attempting trade 7/7</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:48:35.493078</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr"/>
+      <c r="F191" t="inlineStr"/>
+      <c r="G191" t="inlineStr"/>
+      <c r="H191" t="inlineStr"/>
+      <c r="I191" t="inlineStr"/>
+      <c r="J191" t="inlineStr"/>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Thu Jan 15 12:50:09 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L191"/>
+  <dimension ref="A1:L193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8045,6 +8045,84 @@
         </is>
       </c>
     </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2026-01-15T12:50:06.706370</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>0.4145192900403545</v>
+      </c>
+      <c r="F192" t="inlineStr"/>
+      <c r="G192" t="inlineStr"/>
+      <c r="H192" t="inlineStr"/>
+      <c r="I192" t="inlineStr"/>
+      <c r="J192" t="inlineStr"/>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2026-01-15T12:50:08.395180</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr"/>
+      <c r="F193" t="inlineStr"/>
+      <c r="G193" t="inlineStr"/>
+      <c r="H193" t="inlineStr"/>
+      <c r="I193" t="inlineStr"/>
+      <c r="J193" t="inlineStr"/>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trading results - Tue Jan 27 01:56:19 UTC 2026
</commit_message>
<xml_diff>
--- a/results/real_trading_log.xlsx
+++ b/results/real_trading_log.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L193"/>
+  <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,62 +422,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>action</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>signal_type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>position_size_usd</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>leverage</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>stiffness</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>pnl_percent</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>exit_reason</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>error_message</t>
         </is>
@@ -8123,6 +8111,84 @@
         </is>
       </c>
     </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2026-01-27T01:56:17.284403</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>TRADING_ATTEMPT</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>124.2062721119261</v>
+      </c>
+      <c r="F194" t="inlineStr"/>
+      <c r="G194" t="inlineStr"/>
+      <c r="H194" t="inlineStr"/>
+      <c r="I194" t="inlineStr"/>
+      <c r="J194" t="inlineStr"/>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>ATTEMPT</t>
+        </is>
+      </c>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>Attempting trade 1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2026-01-27T01:56:18.665269</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>POSITION_FAILED</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" t="inlineStr"/>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="inlineStr"/>
+      <c r="I195" t="inlineStr"/>
+      <c r="J195" t="inlineStr"/>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>Trade execution failed for trade 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>